<commit_message>
edited mojo_top and all_functions to include new functions
</commit_message>
<xml_diff>
--- a/all_functions.xlsx
+++ b/all_functions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>alufn</t>
   </si>
@@ -146,16 +146,34 @@
     <t>0b111011</t>
   </si>
   <si>
-    <t>DIV</t>
-  </si>
-  <si>
-    <t>MOD</t>
-  </si>
-  <si>
-    <t>0b000100</t>
-  </si>
-  <si>
-    <t>0b000110</t>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>0b100100</t>
+  </si>
+  <si>
+    <t>0b100101</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>0b000011</t>
+  </si>
+  <si>
+    <t>CONST1</t>
+  </si>
+  <si>
+    <t>CONST0</t>
+  </si>
+  <si>
+    <t>0b011111</t>
+  </si>
+  <si>
+    <t>0b010000</t>
   </si>
 </sst>
 </file>
@@ -514,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,145 +574,169 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed CONST1 to CONSTM1
</commit_message>
<xml_diff>
--- a/all_functions.xlsx
+++ b/all_functions.xlsx
@@ -164,9 +164,6 @@
     <t>0b000011</t>
   </si>
   <si>
-    <t>CONST1</t>
-  </si>
-  <si>
     <t>CONST0</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>0b010000</t>
+  </si>
+  <si>
+    <t>CONSTM1</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,18 +646,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bug fixes, added state machine, test cases, more functions
</commit_message>
<xml_diff>
--- a/all_functions.xlsx
+++ b/all_functions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>alufn</t>
   </si>
@@ -107,9 +107,6 @@
     <t>0b010101</t>
   </si>
   <si>
-    <t>0b010111</t>
-  </si>
-  <si>
     <t>0b010001</t>
   </si>
   <si>
@@ -146,18 +143,6 @@
     <t>0b111011</t>
   </si>
   <si>
-    <t>RL</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
-    <t>0b100100</t>
-  </si>
-  <si>
-    <t>0b100101</t>
-  </si>
-  <si>
     <t>ABS</t>
   </si>
   <si>
@@ -174,6 +159,18 @@
   </si>
   <si>
     <t>CONSTM1</t>
+  </si>
+  <si>
+    <t>NOT A</t>
+  </si>
+  <si>
+    <t>NOT B</t>
+  </si>
+  <si>
+    <t>0b011100</t>
+  </si>
+  <si>
+    <t>0b010011</t>
   </si>
 </sst>
 </file>
@@ -535,7 +532,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,10 +571,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,87 +614,87 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,23 +718,23 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected A, B, NOTA, NOTB
</commit_message>
<xml_diff>
--- a/all_functions.xlsx
+++ b/all_functions.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUTD Term 4\50 .002 - LI01 Computation Structures\1D Project\8BitALU\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>alufn</t>
   </si>
@@ -166,12 +171,15 @@
   </si>
   <si>
     <t>0b010111</t>
+  </si>
+  <si>
+    <t>0b010011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -609,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +625,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +633,7 @@
         <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>